<commit_message>
Uploaded into main page Criteria 1-4
</commit_message>
<xml_diff>
--- a/process/uploads/PM Data/template.xlsx
+++ b/process/uploads/PM Data/template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pe-system-local\process\uploads\PM Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39FA0A09-5CF4-4A00-8621-0E941DB94B06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E346E3-C772-4DB1-9104-8A4C0D685288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{6A564FEC-4803-4804-A10F-37B2AD608A6B}"/>
+    <workbookView xWindow="20370" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{6A564FEC-4803-4804-A10F-37B2AD608A6B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PM Tool" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,9 +42,6 @@
     <t>VS Method</t>
   </si>
   <si>
-    <t>Parts Unification (Overall)</t>
-  </si>
-  <si>
     <t>Parts Unification (300X300)</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>Method</t>
+  </si>
+  <si>
+    <t>Parts Unification (Overall Length)</t>
   </si>
 </sst>
 </file>
@@ -879,15 +879,6 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
@@ -913,6 +904,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1276,608 +1276,608 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
     <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="1" t="s">
+      <c r="G1" s="21"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="21"/>
+      <c r="N1" s="22"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="20" t="s">
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="H2" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="21" t="s">
-        <v>10</v>
+      <c r="K2" s="19" t="s">
+        <v>8</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>11</v>
+      <c r="L2" s="17" t="s">
+        <v>6</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="M2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="N2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="7"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="4"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="19"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="18"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="15"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="15"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="18"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="15"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="15"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="18"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="15"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="12"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="18"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="15"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="12"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="18"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="15"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="12"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="18"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="15"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="12"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="18"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="15"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="12"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="18"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="15"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="12"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="18"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="15"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="12"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="18"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="15"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="12"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="18"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="15"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="12"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="18"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="15"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="12"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="18"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="15"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="12"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="18"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="15"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="12"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="18"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="15"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="12"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="18"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="15"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="12"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="18"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="15"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="12"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="18"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="15"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="12"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="18"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="15"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="12"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="18"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="15"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="12"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="18"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="15"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="12"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="18"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="15"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="12"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="18"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="15"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="12"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="18"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="15"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="12"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="18"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="15"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="12"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="18"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="15"/>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="12"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="18"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="15"/>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="12"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="18"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="15"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="12"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="18"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="15"/>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="12"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="18"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="15"/>
     </row>
     <row r="34" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A34" s="6"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="11"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>